<commit_message>
Added more detail to the cheatsheets
</commit_message>
<xml_diff>
--- a/HTML, CSS, JavaScript, TypeScript, Bulma CSS and Tailwind CSS Cheatsheet.xlsx
+++ b/HTML, CSS, JavaScript, TypeScript, Bulma CSS and Tailwind CSS Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDCF6B6-3826-4CFE-A1B2-CE148AB75125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816D41B9-2D03-4B5A-BFA2-CE313F0A0CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="717" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="717" firstSheet="5" activeTab="5" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple HTML" sheetId="8" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="JavaScript Explained" sheetId="12" r:id="rId4"/>
     <sheet name="JavaScript Basics" sheetId="1" r:id="rId5"/>
     <sheet name="JavaScript Intermediate" sheetId="7" r:id="rId6"/>
-    <sheet name="JavaScript HTML Interaction" sheetId="6" r:id="rId7"/>
-    <sheet name="JavaScript Cheeky Things" sheetId="5" r:id="rId8"/>
-    <sheet name="TypeScript Explained" sheetId="3" r:id="rId9"/>
-    <sheet name="All of TypeScript" sheetId="4" r:id="rId10"/>
+    <sheet name="JavaScript Advanced" sheetId="13" r:id="rId7"/>
+    <sheet name="JavaScript HTML Interaction" sheetId="6" r:id="rId8"/>
+    <sheet name="JavaScript Cheeky Things" sheetId="5" r:id="rId9"/>
+    <sheet name="TypeScript Explained" sheetId="3" r:id="rId10"/>
+    <sheet name="All of TypeScript" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="318">
   <si>
     <t>Concept</t>
   </si>
@@ -1959,9 +1960,6 @@
     </r>
   </si>
   <si>
-    <t>HTML input types</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;input type="text" id="username" name="username" placeholder="your name" /&gt;
 </t>
   </si>
@@ -2005,9 +2003,6 @@
   </si>
   <si>
     <t>These are the two ways of adding a normal button to your webpage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding effects to your html document </t>
   </si>
   <si>
     <t>&lt;b&gt;bold&lt;/b&gt;
@@ -2309,6 +2304,77 @@
   </si>
   <si>
     <t>Defer specifies that the script should be executed after the document is loaded in the browser</t>
+  </si>
+  <si>
+    <t>Date: &lt;input type="date" id="dob" name="dob" /&gt;&lt;br /&gt;
+Colour: &lt;input type="color" id="fav-color" name="fav-color" value="#f6b73c" /&gt;</t>
+  </si>
+  <si>
+    <t>Adding effects to your html document text</t>
+  </si>
+  <si>
+    <t>Selection list</t>
+  </si>
+  <si>
+    <t>&lt;select id="fav-fruit" name="fav-fruit"&gt;
+    &lt;option value="none"&gt;&lt;/option&gt;
+    &lt;option value="Apple"&gt;Apple&lt;/option&gt;
+    &lt;option value="Banana"&gt;Banana&lt;/option&gt;
+    &lt;option value="Orange"&gt;Orange&lt;/option&gt;
+    &lt;option value="Grapes"&gt;Grapes&lt;/option&gt;
+    &lt;option value="Pear"&gt;Pear&lt;/option&gt;
+&lt;/select&gt;</t>
+  </si>
+  <si>
+    <t>The selection list adds a drop down menu with a list of inputs for the user to select from.</t>
+  </si>
+  <si>
+    <t>To grab data from the &lt;select&gt;, we grab the data using .value:
+const selectElement = document.getElementById("mySelect");
+  const selectedValue = selectElement.value;
+  console.log("Selected Value:", selectedValue);
+We can also iterate over the values in the list:
+  const options = selectElement.options;
+  for (let i = 0; i &lt; options.length; i++) {
+    if (options[i].selected) {
+      console.log("Selected Option:", options[i].value);
+    }</t>
+  </si>
+  <si>
+    <t>HTML input types explained</t>
+  </si>
+  <si>
+    <t>Different types of HTML input types</t>
+  </si>
+  <si>
+    <t>Check if the value within an input element has changed in any way</t>
+  </si>
+  <si>
+    <t>const username = document.querySelector('#username')
+  username.addEventListener('change', () =&gt; {
+  validateUsername()
+})</t>
+  </si>
+  <si>
+    <t>By using the "change" input, we will be able to look at specific changes made within the program every time the user inputs a letter. For example, if the username can only contain letters, we can check what is being inputted into the text field at every user input with the "change" keyword. If there is a number in the key, then we will do something. Else, do nothing, or something else.</t>
+  </si>
+  <si>
+    <t>List of regular expression components</t>
+  </si>
+  <si>
+    <t>List of String Methods</t>
+  </si>
+  <si>
+    <t>.toLowerCase()
+.toUpperCase()
+.trim()
+.indexOf()
+.slice()
+.concat()
+.replace()
+.includes()
+.search()
+.match()</t>
   </si>
 </sst>
 </file>
@@ -2651,35 +2717,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="82">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="90">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2704,6 +2744,578 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -2826,20 +3438,20 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2970,20 +3582,20 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3116,30 +3728,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3159,498 +3771,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3666,88 +3786,101 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}" name="Table19" displayName="Table19" ref="A1:D22" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
-  <autoFilter ref="A1:D22" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}" name="Table19" displayName="Table19" ref="A1:D24" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
+  <autoFilter ref="A1:D24" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{917F722D-5727-4D2E-AFC1-482F6FBE44D1}" name="Concept" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{9A63E0A9-E8CA-4EC7-A404-B1612D2C4FAB}" name="Code" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{E87C839B-C9E2-4FE0-8B79-53FBF1501C20}" name="Explained" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{6187F8F6-0F15-4805-A509-FB14E0706314}" name="Notes" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{917F722D-5727-4D2E-AFC1-482F6FBE44D1}" name="Concept" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{9A63E0A9-E8CA-4EC7-A404-B1612D2C4FAB}" name="Code" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{E87C839B-C9E2-4FE0-8B79-53FBF1501C20}" name="Explained" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{6187F8F6-0F15-4805-A509-FB14E0706314}" name="Notes" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E25" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}" name="Table2" displayName="Table2" ref="A1:D5" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
+  <autoFilter ref="A1:D5" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{909A7DFE-AF7A-4AEE-B64B-4DFD1577B15C}" name="Concept" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{8C0E44D8-D479-472D-9150-29C9A92B5D3C}" name="Explained" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{1BF832DC-50E8-42B0-98A6-D7D3C3D87754}" name="Notes" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{F8C9EC3F-25A2-4D4C-90B0-3BF5E194A063}" name="Images" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E25" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:E25" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{C6C4CC59-F9BA-49FA-8B0F-D7372B8894D2}" name="Explained" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{936E524D-0762-4E82-A3EF-588C1391A681}" name="Notes" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{400184B0-77C8-40AE-9D2A-88E525B9230C}" name="Images" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{C6C4CC59-F9BA-49FA-8B0F-D7372B8894D2}" name="Explained" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{936E524D-0762-4E82-A3EF-588C1391A681}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{400184B0-77C8-40AE-9D2A-88E525B9230C}" name="Images" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AA406389-4363-4D21-9373-D3D6BD1FCC1B}" name="Table210" displayName="Table210" ref="A1:D5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AA406389-4363-4D21-9373-D3D6BD1FCC1B}" name="Table210" displayName="Table210" ref="A1:D5" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79" tableBorderDxfId="77">
   <autoFilter ref="A1:D5" xr:uid="{AA406389-4363-4D21-9373-D3D6BD1FCC1B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC69128E-E740-472D-B88F-4242AA4B6159}" name="Concept" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{E58B0CD4-D5C2-46BF-9C69-243BECC0F1F8}" name="Code" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{97A0F511-7B53-4D65-A1A7-C0F0F36F5741}" name="Explained" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{01918EA6-D406-4709-9D34-A5651C921650}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{CC69128E-E740-472D-B88F-4242AA4B6159}" name="Concept" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{E58B0CD4-D5C2-46BF-9C69-243BECC0F1F8}" name="Code" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{97A0F511-7B53-4D65-A1A7-C0F0F36F5741}" name="Explained" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{01918EA6-D406-4709-9D34-A5651C921650}" name="Notes" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{05C88060-49D5-4BEE-8174-318059ACE895}" name="Table311" displayName="Table311" ref="A1:D10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{05C88060-49D5-4BEE-8174-318059ACE895}" name="Table311" displayName="Table311" ref="A1:D10" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69">
   <autoFilter ref="A1:D10" xr:uid="{05C88060-49D5-4BEE-8174-318059ACE895}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8A66607B-B23D-4622-B5DE-8D6FC1C274D3}" name="Concept" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7020C8E7-F89B-48C1-A721-597D9C0976CC}" name="Code" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{6E92E2E9-F390-4295-B3A9-38FC4007161D}" name="Explained" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{CECB4B75-722E-4699-9201-CE759EBE3609}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{8A66607B-B23D-4622-B5DE-8D6FC1C274D3}" name="Concept" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{7020C8E7-F89B-48C1-A721-597D9C0976CC}" name="Code" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{6E92E2E9-F390-4295-B3A9-38FC4007161D}" name="Explained" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{CECB4B75-722E-4699-9201-CE759EBE3609}" name="Notes" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{48A45EE1-69C4-4CF6-9CE0-78E2D8ACAC2C}" name="Table4" displayName="Table4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{48A45EE1-69C4-4CF6-9CE0-78E2D8ACAC2C}" name="Table4" displayName="Table4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61">
   <autoFilter ref="A1:D4" xr:uid="{48A45EE1-69C4-4CF6-9CE0-78E2D8ACAC2C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A524034D-0C77-432E-AB29-981942A91C04}" name="Concept" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2A223867-38E9-498A-8932-A7E9446E4265}" name="Code" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{04CC13FA-0EFD-49DE-89F4-30A8786CACE0}" name="Explained" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{732E92E0-D6AC-4363-9B11-3E9D1B395C40}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A524034D-0C77-432E-AB29-981942A91C04}" name="Concept" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{2A223867-38E9-498A-8932-A7E9446E4265}" name="Code" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{04CC13FA-0EFD-49DE-89F4-30A8786CACE0}" name="Explained" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{732E92E0-D6AC-4363-9B11-3E9D1B395C40}" name="Notes" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}" name="Table1" displayName="Table1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}" name="Table1" displayName="Table1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A1:E19" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{090BD192-1D20-47D2-8F6F-5AF92E218BEB}" name="Concept" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{25DDA5F8-4AB0-4AAC-ABCA-BF59415478C2}" name="Code" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{C1DAB56A-CB82-4D25-8492-48FBFC047ECF}" name="Explained" dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{D17684CE-80C0-4E1E-AA09-5D5E6B7F0C8E}" name="Notes" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{AD919A87-3529-4F1F-B0E4-2D6B1AE0970D}" name="Images" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{090BD192-1D20-47D2-8F6F-5AF92E218BEB}" name="Concept" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{25DDA5F8-4AB0-4AAC-ABCA-BF59415478C2}" name="Code" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{C1DAB56A-CB82-4D25-8492-48FBFC047ECF}" name="Explained" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{D17684CE-80C0-4E1E-AA09-5D5E6B7F0C8E}" name="Notes" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{AD919A87-3529-4F1F-B0E4-2D6B1AE0970D}" name="Images" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}" name="Table6" displayName="Table6" ref="A1:D3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="42" headerRowBorderDxfId="46" tableBorderDxfId="47">
-  <autoFilter ref="A1:D3" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46">
+  <autoFilter ref="A1:D5" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0F3FDFA6-C0B0-44D4-A3E0-840CB4125EA5}" name="Concept" dataDxfId="45"/>
     <tableColumn id="2" xr3:uid="{E5C1789B-D4BD-49A8-A647-5E3B73B44ED3}" name="Code" dataDxfId="44"/>
@@ -3759,7 +3892,20 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{906E7E22-D3C5-4D42-9E14-2929FCF8A4F5}" name="Table7" displayName="Table7" ref="A1:D12" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" headerRowBorderDxfId="39" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B0AE499-2931-4BB3-BCFD-146111CA6BCE}" name="Table8" displayName="Table8" ref="A1:D2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
+  <autoFilter ref="A1:D2" xr:uid="{8B0AE499-2931-4BB3-BCFD-146111CA6BCE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{446F590E-B320-4152-B846-5D104AD80C7F}" name="Concept" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E3B5734C-FD0B-4690-BA0B-DD261496DF8C}" name="Code" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C9F243D5-A50B-4123-94E3-7C97CCFDB44D}" name="Explained" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{08FADC0C-6DF0-414C-884C-85ECE8AB0EB9}" name="Notes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{906E7E22-D3C5-4D42-9E14-2929FCF8A4F5}" name="Table7" displayName="Table7" ref="A1:D12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
   <autoFilter ref="A1:D12" xr:uid="{906E7E22-D3C5-4D42-9E14-2929FCF8A4F5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C6DA0F4F-86CA-454B-9367-74200C1104E3}" name="Concept" dataDxfId="38"/>
@@ -3771,28 +3917,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}" name="Table5" displayName="Table5" ref="A1:E3" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}" name="Table5" displayName="Table5" ref="A1:E3" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
   <autoFilter ref="A1:E3" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5BD4F94D-648B-463B-8902-D0F644FE87F3}" name="Concept" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{14C72CE5-A489-43FD-AFF3-A0FE78AA19C3}" name="Code" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{A6E5DF9D-DF1D-460D-B6C1-3BEADF5D82EB}" name="Explained" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{BDC82D61-2448-4A46-91B3-F81B1675A4A6}" name="Notes" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{71675091-7AB6-4A89-8AB9-672035A77241}" name="Images" dataDxfId="66"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}" name="Table2" displayName="Table2" ref="A1:D5" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62">
-  <autoFilter ref="A1:D5" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{909A7DFE-AF7A-4AEE-B64B-4DFD1577B15C}" name="Concept" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{8C0E44D8-D479-472D-9150-29C9A92B5D3C}" name="Explained" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{1BF832DC-50E8-42B0-98A6-D7D3C3D87754}" name="Notes" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{F8C9EC3F-25A2-4D4C-90B0-3BF5E194A063}" name="Images" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{5BD4F94D-648B-463B-8902-D0F644FE87F3}" name="Concept" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{14C72CE5-A489-43FD-AFF3-A0FE78AA19C3}" name="Code" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{A6E5DF9D-DF1D-460D-B6C1-3BEADF5D82EB}" name="Explained" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{BDC82D61-2448-4A46-91B3-F81B1675A4A6}" name="Notes" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{71675091-7AB6-4A89-8AB9-672035A77241}" name="Images" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4095,18 +4228,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4427A192-665E-4022-814A-FD033B770DA7}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="54.5703125" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4321,65 +4454,89 @@
     </row>
     <row r="18" spans="1:4" ht="60">
       <c r="A18" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="C18" s="26" t="s">
         <v>240</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>241</v>
       </c>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" ht="60">
       <c r="A19" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4" ht="135">
       <c r="A20" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="C20" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="D20" s="22" t="s">
         <v>246</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="60">
       <c r="A21" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="C21" s="21" t="s">
         <v>249</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="D21" s="22"/>
     </row>
     <row r="22" spans="1:4" ht="45">
       <c r="A22" s="20" t="s">
-        <v>251</v>
+        <v>305</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
-        <v>253</v>
-      </c>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="165">
+      <c r="A23" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45">
+      <c r="A24" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4390,6 +4547,80 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FF2D82-85A9-4218-B047-8A72B9F1F6B9}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="119" style="4" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="90">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30">
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="195">
+      <c r="A5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E945EC2-D845-46A8-A317-7E66B9F1414A}">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -4790,56 +5021,56 @@
     </row>
     <row r="2" spans="1:4" ht="225">
       <c r="A2" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="D2" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>256</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60">
       <c r="A3" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="D3" s="23" t="s">
         <v>259</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60">
       <c r="A4" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>262</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>264</v>
       </c>
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4" ht="75">
       <c r="A5" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="D5" s="26" t="s">
         <v>266</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4882,111 +5113,111 @@
     </row>
     <row r="2" spans="1:4" ht="75">
       <c r="A2" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>270</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="A3" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>273</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>274</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>275</v>
       </c>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="75">
       <c r="A4" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="D4" s="31" t="s">
         <v>277</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>278</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105">
       <c r="A5" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" ht="75">
       <c r="A6" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="D6" s="23" t="s">
         <v>283</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="120">
       <c r="A7" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" ht="45">
       <c r="A8" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>288</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>290</v>
       </c>
       <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" ht="75">
       <c r="A9" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>291</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>293</v>
       </c>
       <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" ht="105">
       <c r="A10" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>294</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>296</v>
       </c>
       <c r="D10" s="21"/>
     </row>
@@ -5003,7 +5234,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5030,38 +5261,38 @@
     </row>
     <row r="2" spans="1:4" ht="75">
       <c r="A2" s="32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="105">
       <c r="A3" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>300</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>302</v>
       </c>
       <c r="D3" s="32"/>
     </row>
     <row r="4" spans="1:4" ht="60">
       <c r="A4" s="32" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -5337,10 +5568,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC9ADD3-4E6A-4879-8F69-C1769BD09FC4}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5388,6 +5619,26 @@
         <v>167</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="90">
+      <c r="A4" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="150">
+      <c r="A5" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5397,6 +5648,50 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4E3281-67A4-4428-A5E2-A9BEAE583877}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="66.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B58A76-707B-4532-B12E-5EA6CA67203C}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -5559,7 +5854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA02FE4-ACA5-4E50-AF97-9314ECB48709}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -5625,78 +5920,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FF2D82-85A9-4218-B047-8A72B9F1F6B9}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="119" style="4" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="90">
-      <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60">
-      <c r="A3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="195">
-      <c r="A5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Bulma and more JavaScript items to the cheatsheet
</commit_message>
<xml_diff>
--- a/HTML, CSS, JavaScript, TypeScript, Bulma CSS and Tailwind CSS Cheatsheet.xlsx
+++ b/HTML, CSS, JavaScript, TypeScript, Bulma CSS and Tailwind CSS Cheatsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816D41B9-2D03-4B5A-BFA2-CE313F0A0CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A851538-25B0-4A11-817D-51259B72364A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="717" firstSheet="5" activeTab="5" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <sheet name="JavaScript Cheeky Things" sheetId="5" r:id="rId9"/>
     <sheet name="TypeScript Explained" sheetId="3" r:id="rId10"/>
     <sheet name="All of TypeScript" sheetId="4" r:id="rId11"/>
+    <sheet name="Bulma CSS" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,8 +46,40 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="372">
   <si>
     <t>Concept</t>
   </si>
@@ -2365,16 +2398,604 @@
     <t>List of String Methods</t>
   </si>
   <si>
-    <t>.toLowerCase()
-.toUpperCase()
-.trim()
-.indexOf()
-.slice()
-.concat()
-.replace()
-.includes()
-.search()
-.match()</t>
+    <t>What is Bulma?</t>
+  </si>
+  <si>
+    <t>It's extremely easy to make nice looking websites using Bulma. Although it's not as complex as something like Tailwind, it's simplicity means that to create a nice website can take mere minutes rather than hours</t>
+  </si>
+  <si>
+    <t>Bulma is a modern CSS framework based on Flexbox. It is a free and open-source framework that provides a clean and modular structure for building responsive web interfaces.
+One of the key features of Bulma is its simplicity and ease of use. It uses a straightforward syntax with class-based styling, making it intuitive for developers to create layouts and styles without writing custom CSS. Additionally, Bulma is highly customizable and allows developers to modify its appearance and behavior to suit their specific needs.
+Bulma has gained popularity among developers due to its lightweight nature, flexibility, and modern design aesthetic. It is often compared to other CSS frameworks like Bootstrap and Foundation, but its focus on Flexbox and simplicity sets it apart in the landscape of web development tools.
+The design is done within the classes of the particular part of the code that we'd like, instead of within a specific CSS file.</t>
+  </si>
+  <si>
+    <t>Heroes</t>
+  </si>
+  <si>
+    <t>Download bulma into the repository where you're doing the work:
+npm install bulma
+Link required in the &lt;head&gt; section of the code to enable our new kind of design:
+&lt;link rel="stylesheet" href="https://cdn.jsdelivr.net/npm/bulma@0.9.3/css/bulma.min.css"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;section class="hero is-fullheight has-background-black"&gt;
+    &lt;div class="hero-body"&gt;
+        &lt;div class="container"
+…
+        &lt;/div&gt;
+    &lt;/div&gt;
+&lt;/section&gt;</t>
+  </si>
+  <si>
+    <t>Class addons</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;section class="hero</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;: The main two features for the section element is that determining its height, and its colour:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Height: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is-fullheight (full height), is-large (large), is-small (small), is-halfheight, is-fullheight-with-navbar (full height with separate navbar coded separately above it)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Background colour:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is-primary, is-link... etc
+If we want to make an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>image the background</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, we need to add some additional styling:
+in HTML: &lt;section class="hero is-fullheight"&gt;
+in &lt;style&gt; section:
+&lt;style&gt;
+    /* Custom CSS to set background image */
+    .hero.is-fullheight {
+        background-image: url('lava lamp.jpg');
+        background-size: cover;
+        background-position: center;
+    }
+&lt;/style&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>If we want to add a figure (e.g. an image), we can add these using the &lt;figure class="image"&gt; tag at any point in our program. But of course we can add it straight away here.
+We put everything within the hero-body element within the section hero part.</t>
+  </si>
+  <si>
+    <t>The hero section of a website is the main part of the website that is loaded when you go onto a webpage. E.g. the Nissan website, the body usually takes up most of the top of the page when you load it, but it also doesn't the toolbox at the top.
+To create a hero, you first start with the &lt;section&gt; tab, then add class="hero". After this, you create a div between with class="hero-body", and a div below that called using class="container"
+After this you can then add everything within the tagged bit within the container. The hero is able to encompass almost anything else, including "navbar"s and other things.</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>&lt;section class="section"&gt;
+  &lt;div class="container"&gt;
+    &lt;div class="columns"&gt;
+      &lt;div class="column"&gt;
+        Lorem ipsum dolor dolor bills
+      &lt;/div&gt;
+      &lt;div class="column"&gt;
+        Lorem ipsum
+      &lt;/div&gt;
+      &lt;div class="column"&gt;
+        Lorem yorem
+      &lt;/div&gt;
+    &lt;/div&gt;
+  &lt;/div&gt;
+&lt;/section&gt;</t>
+  </si>
+  <si>
+    <t>The columns are contained within a container, which itself is contained with a section. Underneath, you create a div with class="columns", then within this you can create individual columns with class="column". It automatically changes the page based on how many columns you have, and adjust accordingly.
+It's something to look out for: much of what is made is with a div class="container", and then these things can be within &lt;section&gt; tags. Unless it's a specific type of section, then the section class is just "section"</t>
+  </si>
+  <si>
+    <t>Additional items to prettify the website</t>
+  </si>
+  <si>
+    <t>Notification:
+&lt;div class="notification"&gt; … &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Editing text</t>
+  </si>
+  <si>
+    <t>&lt;div class="is-size-5"&gt;
+    Lorem ipsum
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>When we use Bulma within our code, it very often disables a lot of the previous kinds of tags that exist for different types of text sizes. To fix this, we can envelope our text with a &lt;p&gt; tag, and write in total: &lt;p class="is-size-5"&gt;…&lt;/p&gt;, or whatever number we'd like for the size</t>
+  </si>
+  <si>
+    <t>Colours in Bulma</t>
+  </si>
+  <si>
+    <t>is-size-10: changes the text size to 10
+&lt;h1 class="title"&gt;: forces the text to be a title, and writes it differently to other text. If you have your text within a notification, you can edit the text so that it shows up as a title thing within the notification.</t>
+  </si>
+  <si>
+    <t>Including static media elements</t>
+  </si>
+  <si>
+    <t>Notification envelops a portion of the code into a notification-type area. It's a small thing to add, but it can make certain aspects of our website more interesting. Notifications are very similar to cards (shown later), but cards very often are able to hold a lot more information.</t>
+  </si>
+  <si>
+    <t>&lt;div class="column"&gt;
+                    &lt;div class="notification is-primary"&gt;
+                        &lt;div class="media"&gt;
+                            &lt;div class="media-left"&gt;
+                                &lt;figure class="image is-32x32"&gt;
+                                    &lt;img src="logo.png" alt="Logo"&gt;
+                                &lt;/figure&gt;
+                            &lt;/div&gt;
+                            &lt;div class="media-content"&gt;
+                                &lt;p&gt;This is a notification with a logo.&lt;/p&gt;
+                            &lt;/div&gt;
+                        &lt;/div&gt;
+                    &lt;/div&gt;
+                &lt;/div&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Media in this instance is very different to media such as inserting a video, or an image more generally. If we have a card or notification area, and we want to add an icon to the corner for example, there are specific ways of doing it.
+In the example to the left, we are including an icon onto our notifications item (Although we could use card), and we introduce the div with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>class="media"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. This tucks all media elements within.
+Now we can work with the media elements. We add div class=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"media-left"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and then include within this a &lt;figure class=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"image is-32-32"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; to indicate that it's an image, before tucking the &lt;img src="imagelink.png" within it. If we wanted something on the right, like a delete button, we can use class=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"media-right"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and add a button with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>class="delete"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (covered later).
+When we are styling a page using HTML like this, the important thing (and slightly annoying, but ultimately necessary thing) is that everything is layered. The image is layed within the class="image", which is latered withing the "media-left", within "media", withing "column", within "columns", and on, and on. It allows for precision, and for most other programming situations, we're not necessarily dealing with this. Front-end UI, on the other hand, is different.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We have to make certain things specific when adding media:
+&lt;div class="media"&gt; seems normal, but underneath:
+  class="media-left" (forces the media icon to the left), "media-right" (forces the media to the right).
+Underneath this, we add our image within the figure:
+&lt;figure class="image"&gt; &lt;img src="..."&gt;
+We can specify the size of the item by using pre-built dimensions such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-16x16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-32-32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can force the width of each individual column now matter how many are on a single line with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"is-one-third" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">line within the class="column" section. If we have two items, and only do the first one as one-third, the second one will take over the remaining two-thirds.
+If we have more than three columns, all with is-one-third, that we want to continue going down, we can do this in the columns div:
+&lt;div class="columns </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is-multiline"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>For individual items (like notification): is-primary (light green), is-warning (yellow), is-danger (light red), is-link (darker blue), is-info (lighter blue), is-light (cream white), is-black (black), is-white (white)
+For larger sections (such as background or entire hero sections): has-background-primary, …-danger, etc</t>
+  </si>
+  <si>
+    <t>If we want the text from a p tag to be closer to a h1 title tag (hug the title), we can include subtitle in the p tag: &lt;p class="is-size-6 subtitle"&gt; &lt;/p&gt;. Whether we put subtitle first, or specify the size of the text isn't important.</t>
+  </si>
+  <si>
+    <t>When we change the background colour of a notification/card/whatever we're styling, the actual colour of the button changes also, which is a nice feature.
+There is a nice one to remember: the delete button, which you add using &lt;button class="delete"&gt;&lt;/button&gt;
+We have icons from FontAwesome, which allow us to customise the colours very easily and on the fly. Icons are written like this:
+&lt;span class="icon-text"&gt;
+  &lt;span class="icon"&gt;
+    &lt;i class="fas fa-train"&gt;&lt;/i&gt;
+  &lt;/span&gt;
+... but I can't get them to work</t>
+  </si>
+  <si>
+    <t>Get the date</t>
+  </si>
+  <si>
+    <t>const date = new Date();
+showDate(now);
+showTime(now);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To work with the date and time in JavaScript, we have to start by creating a Date object using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new Date();.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> After this, we can grab a number of values from the Date object that we've created by using showDate(dateObject) and showTime(dateObject).</t>
+    </r>
+  </si>
+  <si>
+    <t>Additional functions:
+getHours(), getMinutes(), getSeconds()</t>
+  </si>
+  <si>
+    <t>Spread operator</t>
+  </si>
+  <si>
+    <t>const cat1 = {
+name: "Toby",
+age: 3
+}
+const cat2 = {
+...cat1,
+owner: "Jo"
+}
+console.log(cat2);
+{name: 'Toby', age: 3, owner: 'Jo'}</t>
+  </si>
+  <si>
+    <t>We can use … in order to join up arrays/dictionaries together. It's basically another way of doing concatination, except it's only for Arrays and dictionaries (I think).</t>
+  </si>
+  <si>
+    <t>Rest parameters (for taking an indefinite number of arguments as an array)</t>
+  </si>
+  <si>
+    <t>const sum = (...args) =&gt; {
+  let result = 0
+  args.forEach((arg) =&gt; (result += arg))
+  return result
+}
+console.log(sum(1, 2))
+console.log(sum(1, 2, 3))
+console.log(sum(1, 2, 3, 4, 5))</t>
+  </si>
+  <si>
+    <t>We can also use … before a variable name into a function. This means we can take an indefinite number of arguments into our code, and then we will be able to access those items within an array.</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>const list = [1, 3, 4, 1, 5, 2]
+const unique = new Set(list)
+console.log([...unique]) // [1, 3, 4, 5, 2]
+unique.add(3)</t>
+  </si>
+  <si>
+    <t>We create sets within JavaScript by creating a Set object. We can create it first of all by adding an already existing list into it, and then we can add an item to the Set using .add(3), or whatever it is.</t>
+  </si>
+  <si>
+    <t>const stock = new Map()
+stock.set('Laptop', 20)
+stock.set('Tablet', 50)
+stock.set('PC', 10)</t>
+  </si>
+  <si>
+    <t>Key-value pair</t>
+  </si>
+  <si>
+    <t>Key-Value pair/Map</t>
+  </si>
+  <si>
+    <t>Strict mode</t>
+  </si>
+  <si>
+    <t>use strict'
+const side = 4
+console.log(size) // throws an error</t>
+  </si>
+  <si>
+    <t>To invoke strict mode, we add the statement ‘use strict’ before other
+statements. It helps us write good and secure JS code. E.g. In strict mode, variables must be declared before we can use them</t>
+  </si>
+  <si>
+    <t>Importing and exporting modules</t>
+  </si>
+  <si>
+    <t>Export examples:
+export function add(a, b) {
+  return a + b;
+}
+export default entityName;
+Import examples:
+import { export1, export2, ... } from 'module-name';
+import * as math from './math.js'; // to import all modules and then use later
+console.log(math.add(5, 3)); // Output: 8</t>
+  </si>
+  <si>
+    <t>The foreach code can be understood like this:
+list1.foreach((args) =&gt; (result += arg));
+[for each of the] args [do this] =&gt; result += arg</t>
+  </si>
+  <si>
+    <t>When we are working with many more JavaScript files, one of the key features that we'll need to add is the ability to import and export modules from different files towards one another. It's usually quite easy, as to export we just need to add the keyword export in front of the function/variable. To import is the same as is done in every other type of file, which is using the import module at the top of the code.</t>
+  </si>
+  <si>
+    <t>.toLowerCase() - forces the string to lower case
+.toUpperCase() - forces the string to upper case
+.trim(): Removes whitespace from both ends of a string.
+.indexOf(): Returns the index within the calling string object of the first occurrence of the specified value.
+.slice(): Extracts a section of a string and returns it as a new string.
+.concat(): Combines two or more strings and returns a new string.
+.replace(): Replaces a specified value with another value in a string.
+.includes(): Checks if a string contains the specified value and returns true or false.
+.search(): Searches a string for a specified value and returns the position of the match.
+.match(): Retrieves the matches when matching a string against a regular expression.</t>
+  </si>
+  <si>
+    <t>List of Array methods</t>
+  </si>
+  <si>
+    <t>Array.from: Creates a new array from an array-like or iterable object.
+.includes: Checks if an array contains a certain element and returns true or false.
+.filter: Creates a new array with all elements that pass the test implemented by the provided function.
+.some: Checks if at least one element in the array passes the test implemented by the provided function and returns true or false..
+sort: Sorts the elements of an array in place and returns the sorted array.
+.toSorted: Sorts the elements of an array and returns a new sorted array.
+.join: Joins all elements of an array into a string, separated by the specified separator string.</t>
   </si>
 </sst>
 </file>
@@ -2615,7 +3236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2713,13 +3334,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="100">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2745,31 +3401,15 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3012,6 +3652,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3785,106 +4479,190 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}" name="Table19" displayName="Table19" ref="A1:D24" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}" name="Table19" displayName="Table19" ref="A1:D24" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
   <autoFilter ref="A1:D24" xr:uid="{AD8BB456-CCE1-4CF4-8069-86F2DB79FD28}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{917F722D-5727-4D2E-AFC1-482F6FBE44D1}" name="Concept" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{9A63E0A9-E8CA-4EC7-A404-B1612D2C4FAB}" name="Code" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{E87C839B-C9E2-4FE0-8B79-53FBF1501C20}" name="Explained" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{6187F8F6-0F15-4805-A509-FB14E0706314}" name="Notes" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{917F722D-5727-4D2E-AFC1-482F6FBE44D1}" name="Concept" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{9A63E0A9-E8CA-4EC7-A404-B1612D2C4FAB}" name="Code" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{E87C839B-C9E2-4FE0-8B79-53FBF1501C20}" name="Explained" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{6187F8F6-0F15-4805-A509-FB14E0706314}" name="Notes" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}" name="Table2" displayName="Table2" ref="A1:D5" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}" name="Table2" displayName="Table2" ref="A1:D5" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
   <autoFilter ref="A1:D5" xr:uid="{86A51DF5-045C-430C-8E6C-5414FCA48178}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{909A7DFE-AF7A-4AEE-B64B-4DFD1577B15C}" name="Concept" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{8C0E44D8-D479-472D-9150-29C9A92B5D3C}" name="Explained" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{1BF832DC-50E8-42B0-98A6-D7D3C3D87754}" name="Notes" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{F8C9EC3F-25A2-4D4C-90B0-3BF5E194A063}" name="Images" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{909A7DFE-AF7A-4AEE-B64B-4DFD1577B15C}" name="Concept" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{8C0E44D8-D479-472D-9150-29C9A92B5D3C}" name="Explained" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{1BF832DC-50E8-42B0-98A6-D7D3C3D87754}" name="Notes" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{F8C9EC3F-25A2-4D4C-90B0-3BF5E194A063}" name="Images" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E25" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}" name="Table3" displayName="Table3" ref="A1:E25" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:E25" xr:uid="{D3CF9E49-9401-4255-90C1-990A95C7B43D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{C6C4CC59-F9BA-49FA-8B0F-D7372B8894D2}" name="Explained" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{936E524D-0762-4E82-A3EF-588C1391A681}" name="Notes" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{400184B0-77C8-40AE-9D2A-88E525B9230C}" name="Images" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{3A580996-E5D3-4561-AC07-BA4822C0708C}" name="Concept" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DA354905-1BC8-460D-98B4-ADED2D10AFBF}" name="Code" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{C6C4CC59-F9BA-49FA-8B0F-D7372B8894D2}" name="Explained" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{936E524D-0762-4E82-A3EF-588C1391A681}" name="Notes" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{400184B0-77C8-40AE-9D2A-88E525B9230C}" name="Images" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{724655A1-2430-4A96-8365-DBDB8440D243}" name="Table12" displayName="Table12" ref="A1:F8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:F8" xr:uid="{724655A1-2430-4A96-8365-DBDB8440D243}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{EE5ACA6C-EE94-4E02-8773-B940BE7C1C9A}" name="Concept" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{B7504359-43A5-4883-8237-C303C8CC455F}" name="Code" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{8D6B0FB3-D971-4A80-A21E-EEDD28A3E59B}" name="Explained" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{1550C285-F112-4A3C-ADD0-AA1345C935BF}" name="Class addons" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A750BD9D-FA1E-45C6-82FC-30998AF2AF1F}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D4A67086-DF3D-4AD3-AD09-AC9DDBE11387}" name="Images" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AA406389-4363-4D21-9373-D3D6BD1FCC1B}" name="Table210" displayName="Table210" ref="A1:D5" totalsRowShown="0" headerRowDxfId="80" dataDxfId="78" headerRowBorderDxfId="79" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{AA406389-4363-4D21-9373-D3D6BD1FCC1B}" name="Table210" displayName="Table210" ref="A1:D5" totalsRowShown="0" headerRowDxfId="90" dataDxfId="88" headerRowBorderDxfId="89" tableBorderDxfId="87">
   <autoFilter ref="A1:D5" xr:uid="{AA406389-4363-4D21-9373-D3D6BD1FCC1B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC69128E-E740-472D-B88F-4242AA4B6159}" name="Concept" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{E58B0CD4-D5C2-46BF-9C69-243BECC0F1F8}" name="Code" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{97A0F511-7B53-4D65-A1A7-C0F0F36F5741}" name="Explained" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{01918EA6-D406-4709-9D34-A5651C921650}" name="Notes" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{CC69128E-E740-472D-B88F-4242AA4B6159}" name="Concept" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{E58B0CD4-D5C2-46BF-9C69-243BECC0F1F8}" name="Code" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{97A0F511-7B53-4D65-A1A7-C0F0F36F5741}" name="Explained" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{01918EA6-D406-4709-9D34-A5651C921650}" name="Notes" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{05C88060-49D5-4BEE-8174-318059ACE895}" name="Table311" displayName="Table311" ref="A1:D10" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{05C88060-49D5-4BEE-8174-318059ACE895}" name="Table311" displayName="Table311" ref="A1:D10" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79">
   <autoFilter ref="A1:D10" xr:uid="{05C88060-49D5-4BEE-8174-318059ACE895}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8A66607B-B23D-4622-B5DE-8D6FC1C274D3}" name="Concept" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{7020C8E7-F89B-48C1-A721-597D9C0976CC}" name="Code" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{6E92E2E9-F390-4295-B3A9-38FC4007161D}" name="Explained" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{CECB4B75-722E-4699-9201-CE759EBE3609}" name="Notes" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{8A66607B-B23D-4622-B5DE-8D6FC1C274D3}" name="Concept" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{7020C8E7-F89B-48C1-A721-597D9C0976CC}" name="Code" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{6E92E2E9-F390-4295-B3A9-38FC4007161D}" name="Explained" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{CECB4B75-722E-4699-9201-CE759EBE3609}" name="Notes" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{48A45EE1-69C4-4CF6-9CE0-78E2D8ACAC2C}" name="Table4" displayName="Table4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{48A45EE1-69C4-4CF6-9CE0-78E2D8ACAC2C}" name="Table4" displayName="Table4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="74" dataDxfId="72" headerRowBorderDxfId="73" tableBorderDxfId="71">
   <autoFilter ref="A1:D4" xr:uid="{48A45EE1-69C4-4CF6-9CE0-78E2D8ACAC2C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A524034D-0C77-432E-AB29-981942A91C04}" name="Concept" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{2A223867-38E9-498A-8932-A7E9446E4265}" name="Code" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{04CC13FA-0EFD-49DE-89F4-30A8786CACE0}" name="Explained" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{732E92E0-D6AC-4363-9B11-3E9D1B395C40}" name="Notes" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{A524034D-0C77-432E-AB29-981942A91C04}" name="Concept" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{2A223867-38E9-498A-8932-A7E9446E4265}" name="Code" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{04CC13FA-0EFD-49DE-89F4-30A8786CACE0}" name="Explained" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{732E92E0-D6AC-4363-9B11-3E9D1B395C40}" name="Notes" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}" name="Table1" displayName="Table1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
-  <autoFilter ref="A1:E19" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}" name="Table1" displayName="Table1" ref="A1:E20" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+  <autoFilter ref="A1:E20" xr:uid="{D67A83B5-6DB9-4D1D-B1E1-F7D382D58B3C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{090BD192-1D20-47D2-8F6F-5AF92E218BEB}" name="Concept" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{25DDA5F8-4AB0-4AAC-ABCA-BF59415478C2}" name="Code" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{C1DAB56A-CB82-4D25-8492-48FBFC047ECF}" name="Explained" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{D17684CE-80C0-4E1E-AA09-5D5E6B7F0C8E}" name="Notes" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{AD919A87-3529-4F1F-B0E4-2D6B1AE0970D}" name="Images" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{090BD192-1D20-47D2-8F6F-5AF92E218BEB}" name="Concept" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{25DDA5F8-4AB0-4AAC-ABCA-BF59415478C2}" name="Code" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{C1DAB56A-CB82-4D25-8492-48FBFC047ECF}" name="Explained" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{D17684CE-80C0-4E1E-AA09-5D5E6B7F0C8E}" name="Notes" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{AD919A87-3529-4F1F-B0E4-2D6B1AE0970D}" name="Images" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}" name="Table6" displayName="Table6" ref="A1:D5" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46">
-  <autoFilter ref="A1:D5" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}" name="Table6" displayName="Table6" ref="A1:D8" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56">
+  <autoFilter ref="A1:D8" xr:uid="{D841B14E-B859-4B50-B683-D34CD5815E94}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0F3FDFA6-C0B0-44D4-A3E0-840CB4125EA5}" name="Concept" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{E5C1789B-D4BD-49A8-A647-5E3B73B44ED3}" name="Code" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{1A39EA4F-42DF-49A9-85E2-C6C4EFC3E222}" name="Explained" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{0F3FDFA6-C0B0-44D4-A3E0-840CB4125EA5}" name="Concept" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{E5C1789B-D4BD-49A8-A647-5E3B73B44ED3}" name="Code" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{1A39EA4F-42DF-49A9-85E2-C6C4EFC3E222}" name="Explained" dataDxfId="53"/>
     <tableColumn id="4" xr3:uid="{EF256CD5-7543-46B8-9612-FEBDAF6FB701}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3892,40 +4670,40 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B0AE499-2931-4BB3-BCFD-146111CA6BCE}" name="Table8" displayName="Table8" ref="A1:D2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
-  <autoFilter ref="A1:D2" xr:uid="{8B0AE499-2931-4BB3-BCFD-146111CA6BCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B0AE499-2931-4BB3-BCFD-146111CA6BCE}" name="Table8" displayName="Table8" ref="A1:D3" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49">
+  <autoFilter ref="A1:D3" xr:uid="{8B0AE499-2931-4BB3-BCFD-146111CA6BCE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{446F590E-B320-4152-B846-5D104AD80C7F}" name="Concept" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E3B5734C-FD0B-4690-BA0B-DD261496DF8C}" name="Code" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C9F243D5-A50B-4123-94E3-7C97CCFDB44D}" name="Explained" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{08FADC0C-6DF0-414C-884C-85ECE8AB0EB9}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{446F590E-B320-4152-B846-5D104AD80C7F}" name="Concept" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{E3B5734C-FD0B-4690-BA0B-DD261496DF8C}" name="Code" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{C9F243D5-A50B-4123-94E3-7C97CCFDB44D}" name="Explained" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{08FADC0C-6DF0-414C-884C-85ECE8AB0EB9}" name="Notes" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{906E7E22-D3C5-4D42-9E14-2929FCF8A4F5}" name="Table7" displayName="Table7" ref="A1:D12" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{906E7E22-D3C5-4D42-9E14-2929FCF8A4F5}" name="Table7" displayName="Table7" ref="A1:D12" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
   <autoFilter ref="A1:D12" xr:uid="{906E7E22-D3C5-4D42-9E14-2929FCF8A4F5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C6DA0F4F-86CA-454B-9367-74200C1104E3}" name="Concept" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{5552EC21-32E4-4E89-987F-89D6B319379F}" name="Code" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{67864CD3-E8D5-4D29-B590-3E8A4525DC97}" name="Explained" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{2FBFC1CD-A8F2-4845-AA43-664C0D89D6D7}" name="Notes" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{C6DA0F4F-86CA-454B-9367-74200C1104E3}" name="Concept" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{5552EC21-32E4-4E89-987F-89D6B319379F}" name="Code" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{67864CD3-E8D5-4D29-B590-3E8A4525DC97}" name="Explained" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{2FBFC1CD-A8F2-4845-AA43-664C0D89D6D7}" name="Notes" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}" name="Table5" displayName="Table5" ref="A1:E3" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
-  <autoFilter ref="A1:E3" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33">
+  <autoFilter ref="A1:E7" xr:uid="{8DA0EE61-EBC9-403D-A661-CD311F36AA7F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5BD4F94D-648B-463B-8902-D0F644FE87F3}" name="Concept" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{14C72CE5-A489-43FD-AFF3-A0FE78AA19C3}" name="Code" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{A6E5DF9D-DF1D-460D-B6C1-3BEADF5D82EB}" name="Explained" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{BDC82D61-2448-4A46-91B3-F81B1675A4A6}" name="Notes" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{71675091-7AB6-4A89-8AB9-672035A77241}" name="Images" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{5BD4F94D-648B-463B-8902-D0F644FE87F3}" name="Concept" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{14C72CE5-A489-43FD-AFF3-A0FE78AA19C3}" name="Code" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{A6E5DF9D-DF1D-460D-B6C1-3BEADF5D82EB}" name="Explained" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{BDC82D61-2448-4A46-91B3-F81B1675A4A6}" name="Notes" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{71675091-7AB6-4A89-8AB9-672035A77241}" name="Images" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4230,8 +5008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4427A192-665E-4022-814A-FD033B770DA7}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4414,7 +5192,7 @@
       </c>
       <c r="D14" s="22"/>
     </row>
-    <row r="15" spans="1:4" ht="60">
+    <row r="15" spans="1:4" ht="45">
       <c r="A15" s="20" t="s">
         <v>229</v>
       </c>
@@ -4464,7 +5242,7 @@
       </c>
       <c r="D18" s="22"/>
     </row>
-    <row r="19" spans="1:4" ht="60">
+    <row r="19" spans="1:4" ht="45">
       <c r="A19" s="27" t="s">
         <v>241</v>
       </c>
@@ -4490,7 +5268,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="60">
+    <row r="21" spans="1:4" ht="45">
       <c r="A21" s="25" t="s">
         <v>247</v>
       </c>
@@ -4550,8 +5328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FF2D82-85A9-4218-B047-8A72B9F1F6B9}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4624,8 +5402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E945EC2-D845-46A8-A317-7E66B9F1414A}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4980,6 +5758,157 @@
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2EF682-225A-4BBC-A364-8405683B998C}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="93.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="62.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="83.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="74.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="165">
+      <c r="A2" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="270">
+      <c r="A3" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" s="4" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="225">
+      <c r="A4" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="84.75" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F5" s="4" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75">
+      <c r="A6" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75">
+      <c r="A7" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="210">
+      <c r="A8" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5305,10 +6234,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1248A541-ED2E-47A6-9221-52FC18FFA65E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5558,6 +6487,19 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
+    <row r="20" spans="1:5" ht="60">
+      <c r="A20" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5568,16 +6510,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC9ADD3-4E6A-4879-8F69-C1769BD09FC4}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.5703125" customWidth="1"/>
     <col min="4" max="4" width="50.140625" customWidth="1"/>
   </cols>
@@ -5630,14 +6572,45 @@
         <v>314</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="150">
+    <row r="5" spans="1:4" ht="210">
       <c r="A5" s="4" t="s">
         <v>316</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>317</v>
+        <v>369</v>
       </c>
       <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="60">
+      <c r="A6" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="150">
+      <c r="A7" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="165">
+      <c r="A8" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5652,7 +6625,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5695,8 +6668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B58A76-707B-4532-B12E-5EA6CA67203C}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5856,10 +6829,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA02FE4-ACA5-4E50-AF97-9314ECB48709}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5914,6 +6887,56 @@
         <v>161</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="60">
+      <c r="A4" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="150">
+      <c r="A5" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="120">
+      <c r="A6" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45">
+      <c r="A7" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Added more data to JS
</commit_message>
<xml_diff>
--- a/HTML, CSS, JavaScript, TypeScript, Bulma CSS and Tailwind CSS Cheatsheet.xlsx
+++ b/HTML, CSS, JavaScript, TypeScript, Bulma CSS and Tailwind CSS Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A851538-25B0-4A11-817D-51259B72364A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAE5C56-C3D1-4902-8CF6-934351FE08A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="717" firstSheet="5" activeTab="5" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="717" firstSheet="5" activeTab="6" xr2:uid="{8E0EA162-069A-4055-969A-D163D2934874}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple HTML" sheetId="8" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="376">
   <si>
     <t>Concept</t>
   </si>
@@ -2993,9 +2993,49 @@
 .includes: Checks if an array contains a certain element and returns true or false.
 .filter: Creates a new array with all elements that pass the test implemented by the provided function.
 .some: Checks if at least one element in the array passes the test implemented by the provided function and returns true or false..
-sort: Sorts the elements of an array in place and returns the sorted array.
+.sort: Sorts the elements of an array in place and returns the sorted array.
 .toSorted: Sorts the elements of an array and returns a new sorted array.
 .join: Joins all elements of an array into a string, separated by the specified separator string.</t>
+  </si>
+  <si>
+    <t>const arrayLike = { 0: 'a', 1: 'b', length: 2 };
+const newArray = Array.from(arrayLike); // ['a', 'b']
+const numbers = [1, 2, 3];
+const includesTwo = numbers.includes(2); // true
+const numbers = [1, 2, 3, 4, 5];
+const evens = numbers.filter(number =&gt; number % 2 === 0); // [2, 4]
+const numbers = [1, 2, 3, 4, 5];
+const hasEven = numbers.some(number =&gt; number % 2 === 0); // true
+const numbers = [3, 1, 2];
+const sortedNumbers = numbers.toSorted(); // [1, 2, 3]
+const array = ['Hello', 'world'];
+const joinedString = array.join(' '); // 'Hello world'</t>
+  </si>
+  <si>
+    <t>const sentence = 'The quick brown fox jumps over the lazy dog';
+const index = sentence.indexOf('brown'); // 10
+const str = 'Hello, world';
+const sliced = str.slice(7); // 'world'
+const str = 'Hello, world';
+const replaced = str.replace('world', 'universe'); // 'Hello, universe'
+const str = 'Hello, world';
+const includesWorld = str.includes('world'); // true
+const str = 'Hello, world';
+const position = str.search('world'); // 7
+const str = 'The rain in Spain falls mainly in the plain';
+const matches = str.match(/ain/g); // ['ain', 'ain', 'ain', 'ain']</t>
+  </si>
+  <si>
+    <t>There's quite a lot of regex's in JavaScript, as well as other languages, and the chances are that not all of these will be used all of the time. However, it's good to know some of the top regex's.</t>
+  </si>
+  <si>
+    <t>Top examples:
+[abc] - Matches any of the characters within the brackets
+[^abc} - Matches any character except those within the brackets
+[a-z] - Matches any lowercase letters / [A-Z] - Match any uppercase letters
+\s - Matches any whitespace characters
+\w - Matches any word character (equivalent to [a-zA-Z0-9_])
+\d - Matches any digit character (equivalent to [0-9])</t>
   </si>
 </sst>
 </file>
@@ -6512,8 +6552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC9ADD3-4E6A-4879-8F69-C1769BD09FC4}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="C2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6521,7 +6561,7 @@
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="2" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
+    <col min="4" max="4" width="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6550,7 +6590,7 @@
       </c>
       <c r="D2" s="11"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="90">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="75">
       <c r="A3" s="4" t="s">
         <v>165</v>
       </c>
@@ -6580,6 +6620,9 @@
         <v>369</v>
       </c>
       <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="60">
       <c r="A6" s="4" t="s">
@@ -6603,7 +6646,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="165">
+    <row r="8" spans="1:4" ht="180">
       <c r="A8" s="4" t="s">
         <v>370</v>
       </c>
@@ -6611,6 +6654,9 @@
         <v>371</v>
       </c>
       <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>372</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6624,8 +6670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4E3281-67A4-4428-A5E2-A9BEAE583877}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6633,7 +6679,7 @@
     <col min="1" max="1" width="25.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="66.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" style="4" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -6651,9 +6697,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="105">
       <c r="A2" s="4" t="s">
         <v>315</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>